<commit_message>
Commit #3 (still not done, but getting there)
</commit_message>
<xml_diff>
--- a/FinalProjectVersion2.0/FinalProjectVersion2.0Tests/SampleTerminatedLeasesReport.xlsx
+++ b/FinalProjectVersion2.0/FinalProjectVersion2.0Tests/SampleTerminatedLeasesReport.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Desktop\FinalProgramExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Source\Repos\FinalProjectVersion2.0\FinalProjectVersion2.0\FinalProjectVersion2.0Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="58">
   <si>
     <t>Rent For Terminated Leases Sample Report</t>
   </si>
@@ -188,13 +188,16 @@
     <t>0-55555</t>
   </si>
   <si>
-    <t>SampleAbberviation2</t>
-  </si>
-  <si>
     <t>0-88888</t>
   </si>
   <si>
     <t>0-53451</t>
+  </si>
+  <si>
+    <t>$1,000</t>
+  </si>
+  <si>
+    <t>$2,000</t>
   </si>
 </sst>
 </file>
@@ -202,7 +205,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -255,13 +258,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,8 +619,8 @@
       <c r="D9" s="2">
         <v>42740</v>
       </c>
-      <c r="E9" s="3">
-        <v>1000</v>
+      <c r="E9" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="F9" t="s">
         <v>41</v>
@@ -637,8 +642,8 @@
       <c r="D10" s="2">
         <v>42741</v>
       </c>
-      <c r="E10" s="3">
-        <v>20</v>
+      <c r="E10" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="F10" t="s">
         <v>42</v>
@@ -649,7 +654,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
         <v>22</v>
@@ -660,7 +665,7 @@
       <c r="D11" s="2">
         <v>42743</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="4">
         <v>15</v>
       </c>
       <c r="F11" t="s">
@@ -683,7 +688,7 @@
       <c r="D12" s="2">
         <v>42742</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="4">
         <v>1100</v>
       </c>
       <c r="F12" t="s">
@@ -706,7 +711,7 @@
       <c r="D13" s="2">
         <v>42743</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="4">
         <v>800</v>
       </c>
       <c r="F13" t="s">
@@ -729,7 +734,7 @@
       <c r="D14" s="2">
         <v>42744</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="4">
         <v>1200</v>
       </c>
       <c r="F14" t="s">
@@ -752,7 +757,7 @@
       <c r="D15" s="2">
         <v>42745</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="5">
         <v>1800</v>
       </c>
       <c r="F15" t="s">
@@ -775,11 +780,11 @@
       <c r="D16" s="2">
         <v>42754</v>
       </c>
-      <c r="E16" s="3">
-        <v>1600</v>
+      <c r="E16" s="5">
+        <v>1900</v>
       </c>
       <c r="F16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G16" t="s">
         <v>52</v>
@@ -799,7 +804,7 @@
         <v>42746</v>
       </c>
       <c r="E17" s="3">
-        <v>1600</v>
+        <v>30</v>
       </c>
       <c r="F17" t="s">
         <v>47</v>
@@ -844,7 +849,9 @@
       <c r="D19" s="2">
         <v>42748</v>
       </c>
-      <c r="E19" s="3"/>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
       <c r="F19" t="s">
         <v>49</v>
       </c>
@@ -869,7 +876,7 @@
         <v>800</v>
       </c>
       <c r="F20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G20" t="s">
         <v>52</v>

</xml_diff>